<commit_message>
Updating according TODO list
</commit_message>
<xml_diff>
--- a/data/raw/library.xlsx
+++ b/data/raw/library.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Converter\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0E693-5FDF-4F76-9D62-F98154D88674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>Acentricity</t>
   </si>
@@ -39,25 +48,25 @@
   <si>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
       <t>Mass Density (at 0</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Times New Roman"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
       <t>°</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
       <t>C or 273,15 K or 32°F)</t>
     </r>
@@ -385,28 +394,39 @@
   </si>
   <si>
     <t>E-Benzene</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ω</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,11 +434,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -432,82 +458,78 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -697,21 +719,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,9 +778,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
+      <c r="B2" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
@@ -784,62 +815,62 @@
       </c>
       <c r="M2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="11">
-        <v>0.0114984000101686</v>
+        <v>1.1498400010168599E-2</v>
       </c>
       <c r="C3" s="12">
-        <v>-161.525</v>
+        <v>-161.52500000000001</v>
       </c>
       <c r="D3" s="12">
-        <v>46.4068017578125</v>
+        <v>46.406801757812502</v>
       </c>
       <c r="E3" s="12">
-        <v>-82.4509948730469</v>
+        <v>-82.450994873046895</v>
       </c>
       <c r="F3" s="13">
-        <v>-802.703</v>
+        <v>-802.70299999999997</v>
       </c>
       <c r="G3" s="13">
-        <v>-74.9</v>
+        <v>-74.900000000000006</v>
       </c>
       <c r="H3" s="12">
-        <v>16.0429000854492</v>
+        <v>16.042900085449201</v>
       </c>
       <c r="I3" s="14">
-        <v>0.052</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="J3" s="11">
-        <v>0.71788822328609</v>
+        <v>0.71788822328609003</v>
       </c>
       <c r="K3" s="11">
-        <v>0.010429020769578</v>
+        <v>1.0429020769577999E-2</v>
       </c>
       <c r="L3" s="11">
         <v>14.527360153423</v>
       </c>
       <c r="M3" s="11">
-        <v>1.31427824676826</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1.3142782467682601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="11">
-        <v>0.0986000001430511</v>
+        <v>9.8600000143051106E-2</v>
       </c>
       <c r="C4" s="12">
-        <v>-88.5999969482422</v>
+        <v>-88.599996948242193</v>
       </c>
       <c r="D4" s="12">
         <v>48.8385009765625</v>
       </c>
       <c r="E4" s="12">
-        <v>32.2780090332031</v>
+        <v>32.278009033203098</v>
       </c>
       <c r="F4" s="13">
         <v>-1428.51</v>
@@ -848,25 +879,25 @@
         <v>-84.738</v>
       </c>
       <c r="H4" s="12">
-        <v>30.0699005126953</v>
+        <v>30.069900512695298</v>
       </c>
       <c r="I4" s="14">
-        <v>0.067</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="J4" s="11">
-        <v>1.35625193998807</v>
+        <v>1.3562519399880699</v>
       </c>
       <c r="K4" s="11">
-        <v>0.00862063561869071</v>
+        <v>8.6206356186907095E-3</v>
       </c>
       <c r="L4" s="11">
-        <v>6.35621993563126</v>
+        <v>6.3562199356312599</v>
       </c>
       <c r="M4" s="11">
-        <v>1.20675506891651</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1.2067550689165101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -874,13 +905,13 @@
         <v>0.152400001883507</v>
       </c>
       <c r="C5" s="12">
-        <v>-42.1019958496094</v>
+        <v>-42.101995849609402</v>
       </c>
       <c r="D5" s="12">
-        <v>42.5666015625</v>
+        <v>42.566601562499997</v>
       </c>
       <c r="E5" s="12">
-        <v>96.7480102539063</v>
+        <v>96.748010253906301</v>
       </c>
       <c r="F5" s="13">
         <v>-2044.97</v>
@@ -889,39 +920,39 @@
         <v>-103.89</v>
       </c>
       <c r="H5" s="12">
-        <v>44.0970001220703</v>
+        <v>44.097000122070298</v>
       </c>
       <c r="I5" s="14">
-        <v>0.084</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="J5" s="11">
         <v>2.01026570286158</v>
       </c>
       <c r="K5" s="11">
-        <v>0.00747438743889161</v>
+        <v>7.4743874388916104E-3</v>
       </c>
       <c r="L5" s="11">
-        <v>3.71810921723031</v>
+        <v>3.7181092172303098</v>
       </c>
       <c r="M5" s="11">
         <v>1.14440840771568</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="11">
-        <v>0.184790000319481</v>
+        <v>0.18479000031948101</v>
       </c>
       <c r="C6" s="12">
         <v>-11.7299865722656</v>
       </c>
       <c r="D6" s="12">
-        <v>36.476201171875</v>
+        <v>36.476201171874997</v>
       </c>
       <c r="E6" s="12">
-        <v>134.946008300781</v>
+        <v>134.94600830078099</v>
       </c>
       <c r="F6" s="13">
         <v>-2652.85</v>
@@ -930,39 +961,39 @@
         <v>-134.59</v>
       </c>
       <c r="H6" s="12">
-        <v>58.1240005493164</v>
+        <v>58.124000549316399</v>
       </c>
       <c r="I6" s="14">
         <v>0.1055</v>
       </c>
       <c r="J6" s="11">
-        <v>2.68195413441817</v>
+        <v>2.6819541344181701</v>
       </c>
       <c r="K6" s="11">
-        <v>0.0067971594454823</v>
+        <v>6.7971594454823E-3</v>
       </c>
       <c r="L6" s="11">
-        <v>2.53440555088273</v>
+        <v>2.5344055508827301</v>
       </c>
       <c r="M6" s="11">
         <v>1.11274682088521</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="11">
-        <v>0.20100000500679</v>
+        <v>0.20100000500678999</v>
       </c>
       <c r="C7" s="12">
-        <v>-0.501989746093727</v>
+        <v>-0.50198974609372704</v>
       </c>
       <c r="D7" s="12">
-        <v>37.966201171875</v>
+        <v>37.966201171874999</v>
       </c>
       <c r="E7" s="12">
-        <v>152.049005126953</v>
+        <v>152.04900512695301</v>
       </c>
       <c r="F7" s="13">
         <v>-2659.6</v>
@@ -971,25 +1002,25 @@
         <v>-126.19</v>
       </c>
       <c r="H7" s="12">
-        <v>58.1240005493164</v>
+        <v>58.124000549316399</v>
       </c>
       <c r="I7" s="14">
         <v>0.101400001525879</v>
       </c>
       <c r="J7" s="11">
-        <v>2.68951320777376</v>
+        <v>2.6895132077737598</v>
       </c>
       <c r="K7" s="11">
-        <v>0.00658923046759987</v>
+        <v>6.58923046759987E-3</v>
       </c>
       <c r="L7" s="11">
         <v>2.44997141064575</v>
       </c>
       <c r="M7" s="11">
-        <v>1.11301926156856</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1.1130192615685599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -997,13 +1028,13 @@
         <v>0.222240000963211</v>
       </c>
       <c r="C8" s="12">
-        <v>27.8780151367188</v>
+        <v>27.878015136718801</v>
       </c>
       <c r="D8" s="12">
-        <v>33.3359008789063</v>
+        <v>33.335900878906301</v>
       </c>
       <c r="E8" s="12">
-        <v>187.248010253906</v>
+        <v>187.24801025390599</v>
       </c>
       <c r="F8" s="13">
         <v>-3265.57</v>
@@ -1022,21 +1053,21 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="11">
-        <v>0.253890007734299</v>
+        <v>0.25389000773429898</v>
       </c>
       <c r="C9" s="12">
-        <v>36.0590148925781</v>
+        <v>36.059014892578098</v>
       </c>
       <c r="D9" s="12">
-        <v>33.751201171875</v>
+        <v>33.751201171875003</v>
       </c>
       <c r="E9" s="12">
-        <v>196.450006103516</v>
+        <v>196.45000610351599</v>
       </c>
       <c r="F9" s="13">
         <v>-3273.5</v>
@@ -1055,21 +1086,21 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="11">
-        <v>0.300700008869171</v>
+        <v>0.30070000886917098</v>
       </c>
       <c r="C10" s="12">
-        <v>68.7300048828125</v>
+        <v>68.730004882812494</v>
       </c>
       <c r="D10" s="12">
-        <v>30.316201171875</v>
+        <v>30.316201171875001</v>
       </c>
       <c r="E10" s="12">
-        <v>234.748010253906</v>
+        <v>234.74801025390599</v>
       </c>
       <c r="F10" s="13">
         <v>-3888.5</v>
@@ -1078,31 +1109,31 @@
         <v>-167.29</v>
       </c>
       <c r="H10" s="12">
-        <v>86.1779022216797</v>
+        <v>86.177902221679702</v>
       </c>
       <c r="I10" s="14">
-        <v>0.131600006103516</v>
+        <v>0.13160000610351599</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="11">
-        <v>0.349790006875992</v>
+        <v>0.34979000687599199</v>
       </c>
       <c r="C11" s="12">
-        <v>98.4290100097656</v>
+        <v>98.429010009765605</v>
       </c>
       <c r="D11" s="12">
-        <v>27.3678002929688</v>
+        <v>27.367800292968798</v>
       </c>
       <c r="E11" s="12">
-        <v>267.008020019531</v>
+        <v>267.00802001953099</v>
       </c>
       <c r="F11" s="13">
         <v>-4503.5</v>
@@ -1114,14 +1145,14 @@
         <v>100.205001831055</v>
       </c>
       <c r="I11" s="14">
-        <v>0.1475</v>
+        <v>0.14749999999999999</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1132,10 +1163,10 @@
         <v>125.670007324219</v>
       </c>
       <c r="D12" s="12">
-        <v>24.966201171875</v>
+        <v>24.966201171874999</v>
       </c>
       <c r="E12" s="12">
-        <v>295.448022460938</v>
+        <v>295.44802246093798</v>
       </c>
       <c r="F12" s="13">
         <v>-5118.5</v>
@@ -1144,17 +1175,17 @@
         <v>-208.59</v>
       </c>
       <c r="H12" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I12" s="14">
-        <v>0.1635</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1162,13 +1193,13 @@
         <v>0.445490002632141</v>
       </c>
       <c r="C13" s="12">
-        <v>150.817010498047</v>
+        <v>150.81701049804701</v>
       </c>
       <c r="D13" s="12">
-        <v>23.0007006835937</v>
+        <v>23.000700683593699</v>
       </c>
       <c r="E13" s="12">
-        <v>321.448022460938</v>
+        <v>321.44802246093798</v>
       </c>
       <c r="F13" s="13">
         <v>-5733.55</v>
@@ -1177,22 +1208,22 @@
         <v>-229.19</v>
       </c>
       <c r="H13" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I13" s="14">
-        <v>0.179600006103516</v>
+        <v>0.17960000610351601</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="11">
-        <v>0.488480001688004</v>
+        <v>0.48848000168800398</v>
       </c>
       <c r="C14" s="12">
         <v>174.149011230469</v>
@@ -1201,7 +1232,7 @@
         <v>21.0755004882813</v>
       </c>
       <c r="E14" s="12">
-        <v>344.448022460938</v>
+        <v>344.44802246093798</v>
       </c>
       <c r="F14" s="13">
         <v>-6348.6</v>
@@ -1210,28 +1241,28 @@
         <v>-249.79</v>
       </c>
       <c r="H14" s="12">
-        <v>142.285003662109</v>
+        <v>142.28500366210901</v>
       </c>
       <c r="I14" s="14">
-        <v>0.196</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="11">
-        <v>0.535000026226044</v>
+        <v>0.53500002622604403</v>
       </c>
       <c r="C15" s="12">
-        <v>195.890008544922</v>
+        <v>195.89000854492201</v>
       </c>
       <c r="D15" s="12">
-        <v>19.6493005371094</v>
+        <v>19.649300537109401</v>
       </c>
       <c r="E15" s="12">
         <v>365.149011230469</v>
@@ -1243,7 +1274,7 @@
         <v>-270.49</v>
       </c>
       <c r="H15" s="12">
-        <v>156.313003540039</v>
+        <v>156.31300354003901</v>
       </c>
       <c r="I15" s="14">
         <v>0.212199005126953</v>
@@ -1253,18 +1284,18 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="11">
-        <v>0.561990022659302</v>
+        <v>0.56199002265930198</v>
       </c>
       <c r="C16" s="12">
-        <v>216.278009033203</v>
+        <v>216.27800903320301</v>
       </c>
       <c r="D16" s="12">
-        <v>18.2992004394531</v>
+        <v>18.299200439453099</v>
       </c>
       <c r="E16" s="12">
         <v>385.149011230469</v>
@@ -1273,10 +1304,10 @@
         <v>-7578.66</v>
       </c>
       <c r="G16" s="13">
-        <v>-291.09</v>
+        <v>-291.08999999999997</v>
       </c>
       <c r="H16" s="12">
-        <v>170.339004516602</v>
+        <v>170.33900451660199</v>
       </c>
       <c r="I16" s="14">
         <v>0.228600006103516</v>
@@ -1286,18 +1317,18 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="11">
-        <v>0.623000025749207</v>
+        <v>0.62300002574920699</v>
       </c>
       <c r="C17" s="12">
-        <v>235.429010009766</v>
+        <v>235.42901000976599</v>
       </c>
       <c r="D17" s="12">
-        <v>17.2353002929688</v>
+        <v>17.235300292968802</v>
       </c>
       <c r="E17" s="12">
         <v>402.649011230469</v>
@@ -1309,28 +1340,28 @@
         <v>-311.69</v>
       </c>
       <c r="H17" s="12">
-        <v>184.367004394531</v>
+        <v>184.36700439453099</v>
       </c>
       <c r="I17" s="14">
-        <v>0.244899002075195</v>
+        <v>0.24489900207519499</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="11">
-        <v>0.679000020027161</v>
+        <v>0.67900002002716098</v>
       </c>
       <c r="C18" s="12">
-        <v>253.508020019531</v>
+        <v>253.50802001953099</v>
       </c>
       <c r="D18" s="12">
-        <v>16.2018005371094</v>
+        <v>16.201800537109399</v>
       </c>
       <c r="E18" s="12">
         <v>420.85</v>
@@ -1342,7 +1373,7 @@
         <v>-332.29</v>
       </c>
       <c r="H18" s="12">
-        <v>198.380004882813</v>
+        <v>198.38000488281301</v>
       </c>
       <c r="I18" s="14">
         <v>0.261299011230469</v>
@@ -1352,12 +1383,12 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="11">
-        <v>0.705990016460419</v>
+        <v>0.70599001646041903</v>
       </c>
       <c r="C19" s="12">
         <v>270.618005371094</v>
@@ -1375,25 +1406,25 @@
         <v>-352.99</v>
       </c>
       <c r="H19" s="12">
-        <v>212.410003662109</v>
+        <v>212.41000366210901</v>
       </c>
       <c r="I19" s="14">
-        <v>0.277799011230469</v>
+        <v>0.27779901123046902</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="11">
-        <v>0.764980018138886</v>
+        <v>0.76498001813888605</v>
       </c>
       <c r="C20" s="12">
-        <v>286.790002441406</v>
+        <v>286.79000244140599</v>
       </c>
       <c r="D20" s="12">
         <v>14.2056005859375</v>
@@ -1402,13 +1433,13 @@
         <v>443.85</v>
       </c>
       <c r="F20" s="13">
-        <v>-10038.7</v>
+        <v>-10038.700000000001</v>
       </c>
       <c r="G20" s="13">
         <v>-373.59</v>
       </c>
       <c r="H20" s="12">
-        <v>226.429000854492</v>
+        <v>226.42900085449199</v>
       </c>
       <c r="I20" s="14">
         <v>0.294100006103516</v>
@@ -1418,12 +1449,12 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="11">
-        <v>0.769990026950836</v>
+        <v>0.76999002695083596</v>
       </c>
       <c r="C21" s="12">
         <v>302.149011230469</v>
@@ -1432,7 +1463,7 @@
         <v>13.1690002441406</v>
       </c>
       <c r="E21" s="12">
-        <v>460.219995117188</v>
+        <v>460.21999511718798</v>
       </c>
       <c r="F21" s="13">
         <v>-10653.7</v>
@@ -1441,31 +1472,31 @@
         <v>-394.19</v>
       </c>
       <c r="H21" s="12">
-        <v>240.457000732422</v>
+        <v>240.45700073242199</v>
       </c>
       <c r="I21" s="14">
-        <v>0.310398010253906</v>
+        <v>0.31039801025390601</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="11">
-        <v>0.800000011920929</v>
+        <v>0.80000001192092896</v>
       </c>
       <c r="C22" s="12">
-        <v>316.709008789063</v>
+        <v>316.70900878906298</v>
       </c>
       <c r="D22" s="12">
-        <v>12.1346997070313</v>
+        <v>12.134699707031301</v>
       </c>
       <c r="E22" s="12">
-        <v>472.110009765625</v>
+        <v>472.11000976562502</v>
       </c>
       <c r="F22" s="13">
         <v>-11268.7</v>
@@ -1477,28 +1508,28 @@
         <v>254.47900390625</v>
       </c>
       <c r="I22" s="14">
-        <v>0.326544189453125</v>
+        <v>0.32654418945312502</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="11">
-        <v>0.827000021934509</v>
+        <v>0.82700002193450906</v>
       </c>
       <c r="C23" s="12">
         <v>330.649011230469</v>
       </c>
       <c r="D23" s="12">
-        <v>11.1694995117188</v>
+        <v>11.169499511718801</v>
       </c>
       <c r="E23" s="12">
-        <v>482.779016113281</v>
+        <v>482.77901611328099</v>
       </c>
       <c r="F23" s="13">
         <v>-11883.6</v>
@@ -1517,15 +1548,15 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="11">
-        <v>0.906877994537354</v>
+        <v>0.90687799453735396</v>
       </c>
       <c r="C24" s="12">
-        <v>343.779016113281</v>
+        <v>343.77901611328099</v>
       </c>
       <c r="D24" s="12">
         <v>11.6</v>
@@ -1540,25 +1571,25 @@
         <v>-456.08</v>
       </c>
       <c r="H24" s="12">
-        <v>282.540008544922</v>
+        <v>282.54000854492199</v>
       </c>
       <c r="I24" s="14">
-        <v>0.358470001220703</v>
+        <v>0.35847000122070299</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="11">
-        <v>0.942004024982452</v>
+        <v>0.94200402498245195</v>
       </c>
       <c r="C25" s="12">
-        <v>356.500024414063</v>
+        <v>356.50002441406298</v>
       </c>
       <c r="D25" s="12">
         <v>11.1</v>
@@ -1567,7 +1598,7 @@
         <v>504.85</v>
       </c>
       <c r="F25" s="13">
-        <v>-12960.0</v>
+        <v>-12960</v>
       </c>
       <c r="G25" s="13">
         <v>-477.8</v>
@@ -1576,22 +1607,22 @@
         <v>296.5830078125</v>
       </c>
       <c r="I25" s="14">
-        <v>0.376680480957031</v>
+        <v>0.37668048095703099</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="11">
-        <v>0.972190022468567</v>
+        <v>0.97219002246856701</v>
       </c>
       <c r="C26" s="12">
-        <v>368.610009765625</v>
+        <v>368.61000976562502</v>
       </c>
       <c r="D26" s="12">
         <v>10.6</v>
@@ -1600,94 +1631,94 @@
         <v>513.85</v>
       </c>
       <c r="F26" s="13">
-        <v>-13570.0</v>
+        <v>-13570</v>
       </c>
       <c r="G26" s="13">
         <v>-498.5</v>
       </c>
       <c r="H26" s="12">
-        <v>310.588012695313</v>
+        <v>310.58801269531301</v>
       </c>
       <c r="I26" s="14">
-        <v>0.393599884033203</v>
+        <v>0.39359988403320301</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="11">
-        <v>1.02617001533508</v>
+        <v>1.0261700153350799</v>
       </c>
       <c r="C27" s="12">
-        <v>380.219018554688</v>
+        <v>380.21901855468798</v>
       </c>
       <c r="D27" s="12">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E27" s="12">
         <v>522.85</v>
       </c>
       <c r="F27" s="13">
-        <v>-14170.0</v>
+        <v>-14170</v>
       </c>
       <c r="G27" s="13">
-        <v>-519.2</v>
+        <v>-519.20000000000005</v>
       </c>
       <c r="H27" s="12">
-        <v>324.609008789063</v>
+        <v>324.60900878906301</v>
       </c>
       <c r="I27" s="14">
-        <v>0.410019989013672</v>
+        <v>0.41001998901367198</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="11">
-        <v>1.07102000713348</v>
+        <v>1.0710200071334799</v>
       </c>
       <c r="C28" s="12">
-        <v>391.279016113281</v>
+        <v>391.27901611328099</v>
       </c>
       <c r="D28" s="12">
-        <v>9.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E28" s="12">
         <v>530.85</v>
       </c>
       <c r="F28" s="13">
-        <v>-14790.0</v>
+        <v>-14790</v>
       </c>
       <c r="G28" s="13">
-        <v>-540.0</v>
+        <v>-540</v>
       </c>
       <c r="H28" s="12">
-        <v>338.639007568359</v>
+        <v>338.63900756835898</v>
       </c>
       <c r="I28" s="14">
-        <v>0.427346466064453</v>
+        <v>0.42734646606445298</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B29" s="11">
-        <v>1.105260014534</v>
+        <v>1.1052600145339999</v>
       </c>
       <c r="C29" s="12">
         <v>401.889001464844</v>
@@ -1699,23 +1730,23 @@
         <v>538.85</v>
       </c>
       <c r="F29" s="13">
-        <v>-15390.0</v>
+        <v>-15390</v>
       </c>
       <c r="G29" s="13">
-        <v>-560.7</v>
+        <v>-560.70000000000005</v>
       </c>
       <c r="H29" s="12">
-        <v>352.670013427734</v>
+        <v>352.67001342773398</v>
       </c>
       <c r="I29" s="14">
-        <v>0.444285491943359</v>
+        <v>0.44428549194335898</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>47</v>
       </c>
@@ -1723,7 +1754,7 @@
         <v>1.15444004535675</v>
       </c>
       <c r="C30" s="12">
-        <v>412.219018554688</v>
+        <v>412.21901855468798</v>
       </c>
       <c r="D30" s="12">
         <v>9.1</v>
@@ -1732,13 +1763,13 @@
         <v>545.85</v>
       </c>
       <c r="F30" s="13">
-        <v>-16000.0</v>
+        <v>-16000</v>
       </c>
       <c r="G30" s="13">
         <v>-581.4</v>
       </c>
       <c r="H30" s="12">
-        <v>366.690002441406</v>
+        <v>366.69000244140602</v>
       </c>
       <c r="I30" s="14">
         <v>0.461309692382813</v>
@@ -1748,15 +1779,15 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B31" s="11">
-        <v>1.21356999874115</v>
+        <v>1.2135699987411499</v>
       </c>
       <c r="C31" s="12">
-        <v>422.110009765625</v>
+        <v>422.11000976562502</v>
       </c>
       <c r="D31" s="12">
         <v>8.83</v>
@@ -1765,23 +1796,23 @@
         <v>552.85</v>
       </c>
       <c r="F31" s="13">
-        <v>-16600.0</v>
+        <v>-16600</v>
       </c>
       <c r="G31" s="13">
         <v>-602.1</v>
       </c>
       <c r="H31" s="12">
-        <v>380.720001220703</v>
+        <v>380.72000122070301</v>
       </c>
       <c r="I31" s="14">
-        <v>0.478390655517578</v>
+        <v>0.47839065551757798</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -1789,7 +1820,7 @@
         <v>1.23751997947693</v>
       </c>
       <c r="C32" s="12">
-        <v>431.610009765625</v>
+        <v>431.61000976562502</v>
       </c>
       <c r="D32" s="12">
         <v>8.5</v>
@@ -1798,31 +1829,31 @@
         <v>558.85</v>
       </c>
       <c r="F32" s="13">
-        <v>-17220.0</v>
+        <v>-17220</v>
       </c>
       <c r="G32" s="13">
-        <v>-622.8</v>
+        <v>-622.79999999999995</v>
       </c>
       <c r="H32" s="12">
         <v>394.739013671875</v>
       </c>
       <c r="I32" s="14">
-        <v>0.495608489990234</v>
+        <v>0.49560848999023399</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="11">
-        <v>1.26531004905701</v>
+        <v>1.2653100490570099</v>
       </c>
       <c r="C33" s="12">
-        <v>440.779016113281</v>
+        <v>440.77901611328099</v>
       </c>
       <c r="D33" s="12">
         <v>8.26</v>
@@ -1831,31 +1862,31 @@
         <v>564.85</v>
       </c>
       <c r="F33" s="13">
-        <v>-17820.0</v>
+        <v>-17820</v>
       </c>
       <c r="G33" s="13">
         <v>-643.5</v>
       </c>
       <c r="H33" s="12">
-        <v>408.769012451172</v>
+        <v>408.76901245117199</v>
       </c>
       <c r="I33" s="14">
-        <v>0.513200927734375</v>
+        <v>0.51320092773437498</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="11">
-        <v>1.30718004703522</v>
+        <v>1.3071800470352199</v>
       </c>
       <c r="C34" s="12">
-        <v>449.719018554688</v>
+        <v>449.71901855468798</v>
       </c>
       <c r="D34" s="12">
         <v>8.68</v>
@@ -1864,23 +1895,23 @@
         <v>589.85</v>
       </c>
       <c r="F34" s="13">
-        <v>-18430.0</v>
+        <v>-18430</v>
       </c>
       <c r="G34" s="13">
         <v>-664.2</v>
       </c>
       <c r="H34" s="12">
-        <v>422.799011230469</v>
+        <v>422.79901123046898</v>
       </c>
       <c r="I34" s="14">
-        <v>0.528118896484375</v>
+        <v>0.52811889648437504</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1888,10 +1919,10 @@
         <v>0.196400001645088</v>
       </c>
       <c r="C35" s="12">
-        <v>9.49801025390627</v>
+        <v>9.4980102539062692</v>
       </c>
       <c r="D35" s="12">
-        <v>31.9882006835938</v>
+        <v>31.988200683593799</v>
       </c>
       <c r="E35" s="12">
         <v>160.628015136719</v>
@@ -1906,14 +1937,14 @@
         <v>72.1510009765625</v>
       </c>
       <c r="I35" s="14">
-        <v>0.123300003051758</v>
+        <v>0.12330000305175801</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1921,10 +1952,10 @@
         <v>0.279100000858307</v>
       </c>
       <c r="C36" s="12">
-        <v>60.2610107421875</v>
+        <v>60.261010742187501</v>
       </c>
       <c r="D36" s="12">
-        <v>30.1036010742188</v>
+        <v>30.103601074218801</v>
       </c>
       <c r="E36" s="12">
         <v>224.347009277344</v>
@@ -1936,31 +1967,31 @@
         <v>-174.39</v>
       </c>
       <c r="H36" s="12">
-        <v>86.1779022216797</v>
+        <v>86.177902221679702</v>
       </c>
       <c r="I36" s="14">
-        <v>0.132833465576172</v>
+        <v>0.13283346557617201</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="11">
-        <v>0.275000005960464</v>
+        <v>0.27500000596046398</v>
       </c>
       <c r="C37" s="12">
-        <v>63.2700134277344</v>
+        <v>63.270013427734398</v>
       </c>
       <c r="D37" s="12">
-        <v>31.2384008789063</v>
+        <v>31.238400878906301</v>
       </c>
       <c r="E37" s="12">
-        <v>231.299005126953</v>
+        <v>231.29900512695301</v>
       </c>
       <c r="F37" s="13">
         <v>-3884.05</v>
@@ -1969,31 +2000,31 @@
         <v>-171.69</v>
       </c>
       <c r="H37" s="12">
-        <v>86.1779022216797</v>
+        <v>86.177902221679702</v>
       </c>
       <c r="I37" s="14">
-        <v>0.130631896972656</v>
+        <v>0.13063189697265601</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="11">
-        <v>0.231940001249313</v>
+        <v>0.23194000124931299</v>
       </c>
       <c r="C38" s="12">
-        <v>49.7310119628906</v>
+        <v>49.731011962890598</v>
       </c>
       <c r="D38" s="12">
-        <v>38.806201171875</v>
+        <v>38.806201171875003</v>
       </c>
       <c r="E38" s="12">
-        <v>231.299005126953</v>
+        <v>231.29900512695301</v>
       </c>
       <c r="F38" s="13">
         <v>-3870.08</v>
@@ -2002,31 +2033,31 @@
         <v>-185.69</v>
       </c>
       <c r="H38" s="12">
-        <v>86.1779022216797</v>
+        <v>86.177902221679702</v>
       </c>
       <c r="I38" s="14">
-        <v>0.131944580078125</v>
+        <v>0.13194458007812501</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="11">
-        <v>0.246950000524521</v>
+        <v>0.24695000052452101</v>
       </c>
       <c r="C39" s="12">
-        <v>57.9770141601563</v>
+        <v>57.977014160156301</v>
       </c>
       <c r="D39" s="12">
-        <v>31.268701171875</v>
+        <v>31.268701171875001</v>
       </c>
       <c r="E39" s="12">
-        <v>226.830010986328</v>
+        <v>226.83001098632801</v>
       </c>
       <c r="F39" s="13">
         <v>-3877.9</v>
@@ -2035,31 +2066,31 @@
         <v>-177.89</v>
       </c>
       <c r="H39" s="12">
-        <v>86.1779022216797</v>
+        <v>86.177902221679702</v>
       </c>
       <c r="I39" s="14">
-        <v>0.131112930297852</v>
+        <v>0.13111293029785201</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="11">
-        <v>0.340000003576279</v>
+        <v>0.34000000357627902</v>
       </c>
       <c r="C40" s="12">
-        <v>90.0490051269531</v>
+        <v>90.049005126953105</v>
       </c>
       <c r="D40" s="12">
         <v>27.336201171875</v>
       </c>
       <c r="E40" s="12">
-        <v>257.219018554688</v>
+        <v>257.21901855468798</v>
       </c>
       <c r="F40" s="13">
         <v>-4496.34</v>
@@ -2071,28 +2102,28 @@
         <v>100.205001831055</v>
       </c>
       <c r="I40" s="14">
-        <v>0.14847639465332</v>
+        <v>0.14847639465331999</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B41" s="11">
-        <v>0.326990008354187</v>
+        <v>0.32699000835418701</v>
       </c>
       <c r="C41" s="12">
-        <v>91.8470092773438</v>
+        <v>91.847009277343801</v>
       </c>
       <c r="D41" s="12">
-        <v>28.137900390625</v>
+        <v>28.137900390624999</v>
       </c>
       <c r="E41" s="12">
-        <v>262.1</v>
+        <v>262.10000000000002</v>
       </c>
       <c r="F41" s="13">
         <v>-4498.99</v>
@@ -2111,24 +2142,24 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B42" s="11">
-        <v>0.314000010490417</v>
+        <v>0.31400001049041698</v>
       </c>
       <c r="C42" s="12">
-        <v>93.4720092773438</v>
+        <v>93.472009277343801</v>
       </c>
       <c r="D42" s="12">
-        <v>28.9080004882813</v>
+        <v>28.908000488281299</v>
       </c>
       <c r="E42" s="12">
-        <v>267.490014648438</v>
+        <v>267.49001464843798</v>
       </c>
       <c r="F42" s="13">
-        <v>-4501.61</v>
+        <v>-4501.6099999999997</v>
       </c>
       <c r="G42" s="13">
         <v>-189.79</v>
@@ -2144,18 +2175,18 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B43" s="11">
-        <v>0.300000011920929</v>
+        <v>0.30000001192092901</v>
       </c>
       <c r="C43" s="12">
-        <v>79.1910034179688</v>
+        <v>79.191003417968801</v>
       </c>
       <c r="D43" s="12">
-        <v>27.7326000976562</v>
+        <v>27.732600097656199</v>
       </c>
       <c r="E43" s="12">
         <v>247.35</v>
@@ -2170,31 +2201,31 @@
         <v>100.205001831055</v>
       </c>
       <c r="I43" s="14">
-        <v>0.149445709228516</v>
+        <v>0.14944570922851599</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B44" s="11">
-        <v>0.305000007152557</v>
+        <v>0.30500000715255698</v>
       </c>
       <c r="C44" s="12">
-        <v>89.7780090332031</v>
+        <v>89.778009033203105</v>
       </c>
       <c r="D44" s="12">
         <v>29.0802001953125</v>
       </c>
       <c r="E44" s="12">
-        <v>264.198022460938</v>
+        <v>264.19802246093798</v>
       </c>
       <c r="F44" s="13">
-        <v>-4492.06</v>
+        <v>-4492.0600000000004</v>
       </c>
       <c r="G44" s="13">
         <v>-199.39</v>
@@ -2203,14 +2234,14 @@
         <v>100.205001831055</v>
       </c>
       <c r="I44" s="14">
-        <v>0.143864944458008</v>
+        <v>0.14386494445800799</v>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>62</v>
       </c>
@@ -2218,16 +2249,16 @@
         <v>0.307000011205673</v>
       </c>
       <c r="C45" s="12">
-        <v>80.4930053710938</v>
+        <v>80.493005371093801</v>
       </c>
       <c r="D45" s="12">
-        <v>27.3678002929688</v>
+        <v>27.367800292968798</v>
       </c>
       <c r="E45" s="12">
         <v>246.639001464844</v>
       </c>
       <c r="F45" s="13">
-        <v>-4489.23</v>
+        <v>-4489.2299999999996</v>
       </c>
       <c r="G45" s="13">
         <v>-202.09</v>
@@ -2236,28 +2267,28 @@
         <v>100.205001831055</v>
       </c>
       <c r="I45" s="14">
-        <v>0.149877822875977</v>
+        <v>0.14987782287597701</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B46" s="11">
-        <v>0.287000000476837</v>
+        <v>0.28700000047683699</v>
       </c>
       <c r="C46" s="12">
-        <v>86.0590148925781</v>
+        <v>86.059014892578105</v>
       </c>
       <c r="D46" s="12">
-        <v>29.4551000976562</v>
+        <v>29.455100097656199</v>
       </c>
       <c r="E46" s="12">
-        <v>263.248010253906</v>
+        <v>263.24801025390599</v>
       </c>
       <c r="F46" s="13">
         <v>-4489.76</v>
@@ -2269,31 +2300,31 @@
         <v>100.205001831055</v>
       </c>
       <c r="I46" s="14">
-        <v>0.145350326538086</v>
+        <v>0.14535032653808599</v>
       </c>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B47" s="11">
-        <v>0.259990006685257</v>
+        <v>0.25999000668525701</v>
       </c>
       <c r="C47" s="12">
-        <v>80.8760009765625</v>
+        <v>80.876000976562494</v>
       </c>
       <c r="D47" s="12">
         <v>29.536201171875</v>
       </c>
       <c r="E47" s="12">
-        <v>258.019006347656</v>
+        <v>258.01900634765599</v>
       </c>
       <c r="F47" s="13">
-        <v>-4486.44</v>
+        <v>-4486.4399999999996</v>
       </c>
       <c r="G47" s="13">
         <v>-204.89</v>
@@ -2302,14 +2333,14 @@
         <v>100.205001831055</v>
       </c>
       <c r="I47" s="14">
-        <v>0.146077941894531</v>
+        <v>0.14607794189453099</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>65</v>
       </c>
@@ -2317,46 +2348,46 @@
         <v>0.38400000333786</v>
       </c>
       <c r="C48" s="12">
-        <v>117.653009033203</v>
+        <v>117.65300903320301</v>
       </c>
       <c r="D48" s="12">
-        <v>24.843701171875</v>
+        <v>24.843701171875001</v>
       </c>
       <c r="E48" s="12">
-        <v>286.488000488281</v>
+        <v>286.48800048828099</v>
       </c>
       <c r="F48" s="13">
-        <v>-5111.44</v>
+        <v>-5111.4399999999996</v>
       </c>
       <c r="G48" s="13">
         <v>-215.59</v>
       </c>
       <c r="H48" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I48" s="14">
-        <v>0.164521621704102</v>
+        <v>0.16452162170410201</v>
       </c>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="11">
-        <v>0.368990004062653</v>
+        <v>0.36899000406265298</v>
       </c>
       <c r="C49" s="12">
         <v>118.932000732422</v>
       </c>
       <c r="D49" s="12">
-        <v>25.462900390625</v>
+        <v>25.462900390624998</v>
       </c>
       <c r="E49" s="12">
-        <v>290.519006347656</v>
+        <v>290.51900634765599</v>
       </c>
       <c r="F49" s="13">
         <v>-5114.28</v>
@@ -2365,31 +2396,31 @@
         <v>-212.79</v>
       </c>
       <c r="H49" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I49" s="14">
-        <v>0.162799880981445</v>
+        <v>0.16279988098144499</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="11">
-        <v>0.368990004062653</v>
+        <v>0.36899000406265298</v>
       </c>
       <c r="C50" s="12">
-        <v>117.714013671875</v>
+        <v>117.71401367187499</v>
       </c>
       <c r="D50" s="12">
-        <v>25.421201171875</v>
+        <v>25.421201171875001</v>
       </c>
       <c r="E50" s="12">
-        <v>288.589013671875</v>
+        <v>288.58901367187502</v>
       </c>
       <c r="F50" s="13">
         <v>-5114.83</v>
@@ -2398,7 +2429,7 @@
         <v>-212.19</v>
       </c>
       <c r="H50" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I50" s="14">
         <v>0.162983001708984</v>
@@ -2408,7 +2439,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
@@ -2422,7 +2453,7 @@
         <v>26.0810009765625</v>
       </c>
       <c r="E51" s="12">
-        <v>292.339013671875</v>
+        <v>292.33901367187502</v>
       </c>
       <c r="F51" s="13">
         <v>-5116.08</v>
@@ -2431,7 +2462,7 @@
         <v>-210.99</v>
       </c>
       <c r="H51" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I51" s="14">
         <v>0.153238616943359</v>
@@ -2441,21 +2472,21 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B52" s="11">
-        <v>0.342990010976791</v>
+        <v>0.34299001097679099</v>
       </c>
       <c r="C52" s="12">
         <v>106.842004394531</v>
       </c>
       <c r="D52" s="12">
-        <v>25.2907006835938</v>
+        <v>25.290700683593801</v>
       </c>
       <c r="E52" s="12">
-        <v>276.719018554688</v>
+        <v>276.71901855468798</v>
       </c>
       <c r="F52" s="13">
         <v>-5102.21</v>
@@ -2464,55 +2495,55 @@
         <v>-224.89</v>
       </c>
       <c r="H52" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I52" s="14">
-        <v>0.165217544555664</v>
+        <v>0.16521754455566401</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B53" s="11">
-        <v>0.340000003576279</v>
+        <v>0.34000000357627902</v>
       </c>
       <c r="C53" s="12">
-        <v>115.610009765625</v>
+        <v>115.61000976562499</v>
       </c>
       <c r="D53" s="12">
-        <v>26.283701171875</v>
+        <v>26.283701171874998</v>
       </c>
       <c r="E53" s="12">
-        <v>290.339013671875</v>
+        <v>290.33901367187502</v>
       </c>
       <c r="F53" s="13">
-        <v>-5112.98</v>
+        <v>-5112.9799999999996</v>
       </c>
       <c r="G53" s="13">
         <v>-214.089</v>
       </c>
       <c r="H53" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I53" s="14">
-        <v>0.161269439697266</v>
+        <v>0.16126943969726601</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B54" s="11">
-        <v>0.340990006923676</v>
+        <v>0.34099000692367598</v>
       </c>
       <c r="C54" s="12">
         <v>109.432000732422</v>
@@ -2521,7 +2552,7 @@
         <v>25.563701171875</v>
       </c>
       <c r="E54" s="12">
-        <v>280.37001953125</v>
+        <v>280.37001953125002</v>
       </c>
       <c r="F54" s="13">
         <v>-5107.54</v>
@@ -2530,7 +2561,7 @@
         <v>-219.59</v>
       </c>
       <c r="H54" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I54" s="14">
         <v>0.164014114379883</v>
@@ -2540,12 +2571,12 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B55" s="11">
-        <v>0.345990002155304</v>
+        <v>0.34599000215530401</v>
       </c>
       <c r="C55" s="12">
         <v>109.106011962891</v>
@@ -2563,7 +2594,7 @@
         <v>-222.79</v>
       </c>
       <c r="H55" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I55" s="14">
         <v>0.16543928527832</v>
@@ -2573,12 +2604,12 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B56" s="11">
-        <v>0.32600000500679</v>
+        <v>0.32600000500678999</v>
       </c>
       <c r="C56" s="12">
         <v>111.972009277344</v>
@@ -2587,7 +2618,7 @@
         <v>26.536201171875</v>
       </c>
       <c r="E56" s="12">
-        <v>288.87001953125</v>
+        <v>288.87001953125002</v>
       </c>
       <c r="F56" s="13">
         <v>-5106.79</v>
@@ -2596,7 +2627,7 @@
         <v>-220.29</v>
       </c>
       <c r="H56" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I56" s="14">
         <v>0.151011093139648</v>
@@ -2606,21 +2637,21 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B57" s="11">
-        <v>0.326990008354187</v>
+        <v>0.32699000835418701</v>
       </c>
       <c r="C57" s="12">
-        <v>117.730004882813</v>
+        <v>117.73000488281301</v>
       </c>
       <c r="D57" s="12">
-        <v>26.921201171875</v>
+        <v>26.921201171875001</v>
       </c>
       <c r="E57" s="12">
-        <v>295.698022460938</v>
+        <v>295.69802246093798</v>
       </c>
       <c r="F57" s="13">
         <v>-5113.95</v>
@@ -2629,61 +2660,61 @@
         <v>-213.09</v>
       </c>
       <c r="H57" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I57" s="14">
-        <v>0.159622589111328</v>
+        <v>0.15962258911132801</v>
       </c>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B58" s="11">
-        <v>0.340000003576279</v>
+        <v>0.34000000357627902</v>
       </c>
       <c r="C58" s="12">
-        <v>115.653009033203</v>
+        <v>115.65300903320301</v>
       </c>
       <c r="D58" s="12">
-        <v>27.0031005859375</v>
+        <v>27.003100585937499</v>
       </c>
       <c r="E58" s="12">
-        <v>293.938012695313</v>
+        <v>293.93801269531298</v>
       </c>
       <c r="F58" s="13">
         <v>-5115.75</v>
       </c>
       <c r="G58" s="13">
-        <v>-211.289</v>
+        <v>-211.28899999999999</v>
       </c>
       <c r="H58" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I58" s="14">
-        <v>0.150187973022461</v>
+        <v>0.15018797302246101</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B59" s="11">
-        <v>0.291990011930466</v>
+        <v>0.29199001193046598</v>
       </c>
       <c r="C59" s="12">
         <v>118.265008544922</v>
       </c>
       <c r="D59" s="12">
-        <v>28.076201171875</v>
+        <v>28.076201171874999</v>
       </c>
       <c r="E59" s="12">
         <v>303.430017089844</v>
@@ -2695,31 +2726,31 @@
         <v>-215.09</v>
       </c>
       <c r="H59" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I59" s="14">
-        <v>0.154447250366211</v>
+        <v>0.15444725036621099</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="11">
-        <v>0.296990007162094</v>
+        <v>0.29699000716209401</v>
       </c>
       <c r="C60" s="12">
         <v>109.843011474609</v>
       </c>
       <c r="D60" s="12">
-        <v>27.296201171875</v>
+        <v>27.296201171875001</v>
       </c>
       <c r="E60" s="12">
-        <v>290.35</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="F60" s="13">
         <v>-5106.83</v>
@@ -2728,7 +2759,7 @@
         <v>-220.29</v>
       </c>
       <c r="H60" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I60" s="14">
         <v>0.160350433349609</v>
@@ -2738,21 +2769,21 @@
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B61" s="11">
-        <v>0.310000002384186</v>
+        <v>0.31000000238418601</v>
       </c>
       <c r="C61" s="12">
-        <v>99.2380004882813</v>
+        <v>99.238000488281301</v>
       </c>
       <c r="D61" s="12">
-        <v>25.6757006835938</v>
+        <v>25.675700683593799</v>
       </c>
       <c r="E61" s="12">
-        <v>270.810021972656</v>
+        <v>270.81002197265599</v>
       </c>
       <c r="F61" s="13">
         <v>-5102.75</v>
@@ -2761,28 +2792,28 @@
         <v>-224.29</v>
       </c>
       <c r="H61" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I61" s="14">
-        <v>0.16588899230957</v>
+        <v>0.16588899230956999</v>
       </c>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B62" s="11">
-        <v>0.28999000787735</v>
+        <v>0.28999000787735002</v>
       </c>
       <c r="C62" s="12">
         <v>114.764001464844</v>
       </c>
       <c r="D62" s="12">
-        <v>28.198701171875</v>
+        <v>28.198701171875001</v>
       </c>
       <c r="E62" s="12">
         <v>300.409020996094</v>
@@ -2794,31 +2825,31 @@
         <v>-216.59</v>
       </c>
       <c r="H62" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I62" s="14">
-        <v>0.158093292236328</v>
+        <v>0.15809329223632801</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B63" s="11">
-        <v>0.319990009069443</v>
+        <v>0.31999000906944303</v>
       </c>
       <c r="C63" s="12">
         <v>113.472009277344</v>
       </c>
       <c r="D63" s="12">
-        <v>27.296201171875</v>
+        <v>27.296201171875001</v>
       </c>
       <c r="E63" s="12">
-        <v>293.258020019531</v>
+        <v>293.25802001953099</v>
       </c>
       <c r="F63" s="13">
         <v>-5109.46</v>
@@ -2827,17 +2858,17 @@
         <v>-217.59</v>
       </c>
       <c r="H63" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I63" s="14">
-        <v>0.159679290771484</v>
+        <v>0.15967929077148399</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>81</v>
       </c>
@@ -2848,40 +2879,40 @@
         <v>106.468011474609</v>
       </c>
       <c r="D64" s="12">
-        <v>28.673701171875</v>
+        <v>28.673701171874999</v>
       </c>
       <c r="E64" s="12">
-        <v>294.800012207031</v>
+        <v>294.80001220703099</v>
       </c>
       <c r="F64" s="13">
-        <v>5101.0</v>
+        <v>5101</v>
       </c>
       <c r="G64" s="13">
         <v>-225.89</v>
       </c>
       <c r="H64" s="12">
-        <v>114.232002258301</v>
+        <v>114.23200225830099</v>
       </c>
       <c r="I64" s="14">
-        <v>0.157943542480469</v>
+        <v>0.15794354248046899</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B65" s="11">
-        <v>0.337980002164841</v>
+        <v>0.33798000216484098</v>
       </c>
       <c r="C65" s="12">
-        <v>146.184014892578</v>
+        <v>146.18401489257801</v>
       </c>
       <c r="D65" s="12">
-        <v>26.748701171875</v>
+        <v>26.748701171874998</v>
       </c>
       <c r="E65" s="12">
         <v>336.899011230469</v>
@@ -2893,17 +2924,17 @@
         <v>-232.09</v>
       </c>
       <c r="H65" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I65" s="14">
-        <v>0.169457015991211</v>
+        <v>0.16945701599121099</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>83</v>
       </c>
@@ -2911,13 +2942,13 @@
         <v>0.416680008172989</v>
       </c>
       <c r="C66" s="12">
-        <v>143.278009033203</v>
+        <v>143.27800903320301</v>
       </c>
       <c r="D66" s="12">
         <v>22.898701171875</v>
       </c>
       <c r="E66" s="12">
-        <v>313.6</v>
+        <v>313.60000000000002</v>
       </c>
       <c r="F66" s="13">
         <v>-5679.1</v>
@@ -2926,50 +2957,50 @@
         <v>-229.19</v>
       </c>
       <c r="H66" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I66" s="14">
-        <v>0.180737838745117</v>
+        <v>0.18073783874511701</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B67" s="11">
-        <v>0.418440014123917</v>
+        <v>0.41844001412391701</v>
       </c>
       <c r="C67" s="12">
-        <v>144.230004882813</v>
+        <v>144.23000488281301</v>
       </c>
       <c r="D67" s="12">
-        <v>23.4060009765625</v>
+        <v>23.406000976562499</v>
       </c>
       <c r="E67" s="12">
-        <v>317.000024414063</v>
+        <v>317.00002441406298</v>
       </c>
       <c r="F67" s="13">
         <v>-5681.1</v>
       </c>
       <c r="G67" s="13">
-        <v>-233.717</v>
+        <v>-233.71700000000001</v>
       </c>
       <c r="H67" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I67" s="14">
-        <v>0.179243545532227</v>
+        <v>0.17924354553222699</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>85</v>
       </c>
@@ -2977,22 +3008,22 @@
         <v>0.415100008249283</v>
       </c>
       <c r="C68" s="12">
-        <v>142.438012695313</v>
+        <v>142.43801269531301</v>
       </c>
       <c r="D68" s="12">
-        <v>23.4060009765625</v>
+        <v>23.406000976562499</v>
       </c>
       <c r="E68" s="12">
-        <v>314.500024414063</v>
+        <v>314.50002441406298</v>
       </c>
       <c r="F68" s="13">
         <v>-5680.1</v>
       </c>
       <c r="G68" s="13">
-        <v>-235.224</v>
+        <v>-235.22399999999999</v>
       </c>
       <c r="H68" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I68" s="14">
         <v>0.179255157470703</v>
@@ -3002,28 +3033,28 @@
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B69" s="11">
-        <v>0.416150003671646</v>
+        <v>0.41615000367164601</v>
       </c>
       <c r="C69" s="12">
-        <v>142.998010253906</v>
+        <v>142.99801025390599</v>
       </c>
       <c r="D69" s="12">
-        <v>24.013701171875</v>
+        <v>24.013701171874999</v>
       </c>
       <c r="E69" s="12">
         <v>317.399011230469</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="13">
-        <v>-231.456</v>
+        <v>-231.45599999999999</v>
       </c>
       <c r="H69" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I69" s="14">
         <v>0.17745849609375</v>
@@ -3033,193 +3064,193 @@
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B70" s="11">
-        <v>0.412800014019012</v>
+        <v>0.41280001401901201</v>
       </c>
       <c r="C70" s="12">
-        <v>141.196008300781</v>
+        <v>141.19600830078099</v>
       </c>
       <c r="D70" s="12">
-        <v>23.9126000976563</v>
+        <v>23.912600097656298</v>
       </c>
       <c r="E70" s="12">
-        <v>314.800012207031</v>
+        <v>314.80001220703099</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="13">
         <v>-231.75</v>
       </c>
       <c r="H70" s="12">
-        <v>128.259002685547</v>
+        <v>128.25900268554699</v>
       </c>
       <c r="I70" s="14">
-        <v>0.17732080078125</v>
+        <v>0.17732080078125001</v>
       </c>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B71" s="11">
-        <v>-0.39003199338913</v>
+        <v>-0.39003199338913003</v>
       </c>
       <c r="C71" s="12">
-        <v>-268.940009975433</v>
+        <v>-268.94000997543299</v>
       </c>
       <c r="D71" s="12">
-        <v>2.2697</v>
+        <v>2.2696999999999998</v>
       </c>
       <c r="E71" s="12">
-        <v>-267.96</v>
+        <v>-267.95999999999998</v>
       </c>
       <c r="F71" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G71" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H71" s="12">
-        <v>4.00298023223877</v>
+        <v>4.0029802322387704</v>
       </c>
       <c r="I71" s="14">
-        <v>0.0322654457092285</v>
+        <v>3.2265445709228499E-2</v>
       </c>
       <c r="J71" s="11">
-        <v>0.178572347541496</v>
+        <v>0.17857234754149601</v>
       </c>
       <c r="K71" s="11">
-        <v>0.0597565667202601</v>
+        <v>5.9756566720260099E-2</v>
       </c>
       <c r="L71" s="11">
-        <v>334.635051523719</v>
+        <v>334.63505152371903</v>
       </c>
       <c r="M71" s="11">
         <v>1.66620421037296</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B72" s="11">
-        <v>-0.120090000331402</v>
+        <v>-0.12009000033140201</v>
       </c>
       <c r="C72" s="12">
-        <v>-252.595199966431</v>
+        <v>-252.59519996643101</v>
       </c>
       <c r="D72" s="12">
-        <v>13.155</v>
+        <v>13.154999999999999</v>
       </c>
       <c r="E72" s="12">
         <v>-239.71</v>
       </c>
       <c r="F72" s="13">
-        <v>-241.942</v>
+        <v>-241.94200000000001</v>
       </c>
       <c r="G72" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H72" s="12">
-        <v>2.01600003242493</v>
+        <v>2.0160000324249299</v>
       </c>
       <c r="I72" s="14">
-        <v>0.031</v>
+        <v>3.1E-2</v>
       </c>
       <c r="J72" s="11">
-        <v>0.089899819312379</v>
+        <v>8.9899819312379003E-2</v>
       </c>
       <c r="K72" s="11">
-        <v>0.00808013214465229</v>
+        <v>8.0801321446522904E-3</v>
       </c>
       <c r="L72" s="11">
-        <v>89.879292377395</v>
+        <v>89.879292377395004</v>
       </c>
       <c r="M72" s="11">
         <v>1.41492870277826</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B73" s="11">
-        <v>0.0930000022053719</v>
+        <v>9.3000002205371898E-2</v>
       </c>
       <c r="C73" s="12">
-        <v>-191.450399780273</v>
+        <v>-191.45039978027299</v>
       </c>
       <c r="D73" s="12">
-        <v>34.9875</v>
+        <v>34.987499999999997</v>
       </c>
       <c r="E73" s="12">
-        <v>-140.200994873047</v>
+        <v>-140.20099487304699</v>
       </c>
       <c r="F73" s="13">
-        <v>-283.0</v>
+        <v>-283</v>
       </c>
       <c r="G73" s="13">
         <v>-110.59</v>
       </c>
       <c r="H73" s="12">
-        <v>28.0109004974365</v>
+        <v>28.010900497436499</v>
       </c>
       <c r="I73" s="14">
-        <v>0.0352000007629395</v>
+        <v>3.5200000762939498E-2</v>
       </c>
       <c r="J73" s="11">
-        <v>1.25071686531439</v>
+        <v>1.2507168653143901</v>
       </c>
       <c r="K73" s="11">
-        <v>0.0170105305119752</v>
+        <v>1.7010530511975201E-2</v>
       </c>
       <c r="L73" s="11">
-        <v>13.6006245567811</v>
+        <v>13.600624556781099</v>
       </c>
       <c r="M73" s="11">
         <v>1.40393436598873</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B74" s="11">
-        <v>0.238940000534058</v>
+        <v>0.23894000053405801</v>
       </c>
       <c r="C74" s="12">
-        <v>-78.5519927978515</v>
+        <v>-78.551992797851497</v>
       </c>
       <c r="D74" s="12">
         <v>73.7</v>
       </c>
       <c r="E74" s="12">
-        <v>30.9500061035156</v>
+        <v>30.950006103515602</v>
       </c>
       <c r="F74" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G74" s="13">
         <v>-393.79</v>
       </c>
       <c r="H74" s="12">
-        <v>44.0097007751465</v>
+        <v>44.009700775146499</v>
       </c>
       <c r="I74" s="14">
-        <v>0.044</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="J74" s="11">
-        <v>1.97783830203412</v>
+        <v>1.9778383020341199</v>
       </c>
       <c r="K74" s="11">
-        <v>0.0132747009962592</v>
+        <v>1.3274700996259201E-2</v>
       </c>
       <c r="L74" s="11">
         <v>6.711722076879</v>
@@ -3228,97 +3259,97 @@
         <v>1.2930008334506</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B75" s="11">
-        <v>0.0399998016655445</v>
+        <v>3.9999801665544503E-2</v>
       </c>
       <c r="C75" s="12">
-        <v>-195.800199890137</v>
+        <v>-195.80019989013701</v>
       </c>
       <c r="D75" s="12">
-        <v>33.943701171875</v>
+        <v>33.943701171874999</v>
       </c>
       <c r="E75" s="12">
-        <v>-146.955999755859</v>
+        <v>-146.95599975585901</v>
       </c>
       <c r="F75" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G75" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H75" s="12">
         <v>28.0130004882813</v>
       </c>
       <c r="I75" s="14">
-        <v>0.052</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="J75" s="11">
         <v>1.25077535441775</v>
       </c>
       <c r="K75" s="11">
-        <v>0.017149845282044</v>
+        <v>1.7149845282044E-2</v>
       </c>
       <c r="L75" s="11">
-        <v>13.7113712877941</v>
+        <v>13.711371287794099</v>
       </c>
       <c r="M75" s="11">
-        <v>1.40428601834277</v>
-      </c>
-    </row>
-    <row r="76">
+        <v>1.4042860183427699</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B76" s="11">
-        <v>0.0189999006688595</v>
+        <v>1.8999900668859499E-2</v>
       </c>
       <c r="C76" s="12">
-        <v>-182.950399780273</v>
+        <v>-182.95039978027299</v>
       </c>
       <c r="D76" s="12">
-        <v>50.8002001953125</v>
+        <v>50.800200195312499</v>
       </c>
       <c r="E76" s="12">
         <v>-118.379995727539</v>
       </c>
       <c r="F76" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G76" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H76" s="12">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="I76" s="14">
-        <v>0.0283999004364014</v>
+        <v>2.83999004364014E-2</v>
       </c>
       <c r="J76" s="11">
-        <v>1.42959332056422</v>
+        <v>1.4295933205642199</v>
       </c>
       <c r="K76" s="11">
-        <v>0.019476410879947</v>
+        <v>1.9476410879947E-2</v>
       </c>
       <c r="L76" s="11">
         <v>13.6237422208017</v>
       </c>
       <c r="M76" s="11">
-        <v>1.40647655750543</v>
-      </c>
-    </row>
-    <row r="77">
+        <v>1.4064765575054301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B77" s="11">
-        <v>0.34400001168251</v>
+        <v>0.34400001168250999</v>
       </c>
       <c r="C77" s="12">
-        <v>99.9980102539063</v>
+        <v>99.998010253906301</v>
       </c>
       <c r="D77" s="12">
         <v>221.2</v>
@@ -3327,119 +3358,119 @@
         <v>374.149011230469</v>
       </c>
       <c r="F77" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G77" s="13">
-        <v>-241.814</v>
+        <v>-241.81399999999999</v>
       </c>
       <c r="H77" s="12">
-        <v>18.015100479126</v>
+        <v>18.015100479126001</v>
       </c>
       <c r="I77" s="14">
-        <v>0.0178833827972412</v>
+        <v>1.78833827972412E-2</v>
       </c>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B78" s="11">
-        <v>-0.00400000018998981</v>
+        <v>-4.0000001899898104E-3</v>
       </c>
       <c r="C78" s="12">
-        <v>-185.85059967041</v>
+        <v>-185.85059967040999</v>
       </c>
       <c r="D78" s="12">
-        <v>48.6360009765625</v>
+        <v>48.636000976562499</v>
       </c>
       <c r="E78" s="12">
         <v>-122.442999267578</v>
       </c>
       <c r="F78" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G78" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H78" s="12">
-        <v>39.9480018615723</v>
+        <v>39.948001861572301</v>
       </c>
       <c r="I78" s="14">
-        <v>0.029155294418335</v>
+        <v>2.9155294418335E-2</v>
       </c>
       <c r="J78" s="11">
         <v>1.78464938685799</v>
       </c>
       <c r="K78" s="11">
-        <v>0.0215591693882845</v>
+        <v>2.1559169388284501E-2</v>
       </c>
       <c r="L78" s="11">
         <v>12.0803388873156</v>
       </c>
       <c r="M78" s="11">
-        <v>1.67117782169181</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>1.6711778216918101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B79" s="11">
-        <v>0.0810000002384186</v>
+        <v>8.1000000238418607E-2</v>
       </c>
       <c r="C79" s="12">
         <v>-59.6519989013672</v>
       </c>
       <c r="D79" s="12">
-        <v>90.077900390625</v>
+        <v>90.077900390625004</v>
       </c>
       <c r="E79" s="12">
         <v>100.450006103516</v>
       </c>
       <c r="F79" s="13">
-        <v>-518.0</v>
+        <v>-518</v>
       </c>
       <c r="G79" s="13">
-        <v>-20.179</v>
+        <v>-20.178999999999998</v>
       </c>
       <c r="H79" s="12">
-        <v>34.0808982849121</v>
+        <v>34.080898284912102</v>
       </c>
       <c r="I79" s="14">
-        <v>0.0430998001098633</v>
+        <v>4.30998001098633E-2</v>
       </c>
       <c r="J79" s="11">
         <v>1.53580277230085</v>
       </c>
       <c r="K79" s="11">
-        <v>0.0109770044194915</v>
+        <v>1.0977004419491501E-2</v>
       </c>
       <c r="L79" s="11">
-        <v>7.14740500373392</v>
+        <v>7.1474050037339198</v>
       </c>
       <c r="M79" s="11">
         <v>1.33331522794557</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B80" s="11">
-        <v>0.556990027427673</v>
+        <v>0.55699002742767301</v>
       </c>
       <c r="C80" s="12">
-        <v>64.6490112304688</v>
+        <v>64.649011230468801</v>
       </c>
       <c r="D80" s="12">
-        <v>73.764501953125</v>
+        <v>73.764501953125006</v>
       </c>
       <c r="E80" s="12">
-        <v>239.448022460938</v>
+        <v>239.44802246093801</v>
       </c>
       <c r="F80" s="13">
         <v>-638.1</v>
@@ -3448,28 +3479,28 @@
         <v>-201.29</v>
       </c>
       <c r="H80" s="12">
-        <v>32.0419006347656</v>
+        <v>32.041900634765597</v>
       </c>
       <c r="I80" s="14">
-        <v>0.0407628593444824</v>
+        <v>4.0762859344482399E-2</v>
       </c>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B81" s="11">
-        <v>0.25499901175499</v>
+        <v>0.25499901175499001</v>
       </c>
       <c r="C81" s="12">
-        <v>-33.4509948730469</v>
+        <v>-33.450994873046902</v>
       </c>
       <c r="D81" s="12">
-        <v>112.76900390625</v>
+        <v>112.76900390625001</v>
       </c>
       <c r="E81" s="12">
         <v>132.399011230469</v>
@@ -3481,33 +3512,33 @@
         <v>-45.71</v>
       </c>
       <c r="H81" s="12">
-        <v>17.0300006866455</v>
+        <v>17.030000686645501</v>
       </c>
       <c r="I81" s="14">
-        <v>0.0284598007202148</v>
+        <v>2.8459800720214801E-2</v>
       </c>
       <c r="J81" s="11">
-        <v>0.768031611770952</v>
+        <v>0.76803161177095203</v>
       </c>
       <c r="K81" s="11">
-        <v>0.00758963196900242</v>
+        <v>7.5896319690024203E-3</v>
       </c>
       <c r="L81" s="11">
-        <v>9.88192654141151</v>
+        <v>9.8819265414115094</v>
       </c>
       <c r="M81" s="11">
         <v>1.32093265386183</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B82" s="11">
-        <v>-0.0289999004453421</v>
+        <v>-2.8999900445342099E-2</v>
       </c>
       <c r="C82" s="12">
-        <v>-246.050199890137</v>
+        <v>-246.05019989013701</v>
       </c>
       <c r="D82" s="12">
         <v>27.6</v>
@@ -3516,63 +3547,63 @@
         <v>-228.750299835205</v>
       </c>
       <c r="F82" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G82" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H82" s="12">
-        <v>20.1830005645752</v>
+        <v>20.183000564575199</v>
       </c>
       <c r="I82" s="14">
-        <v>0.0167956523895264</v>
+        <v>1.6795652389526398E-2</v>
       </c>
       <c r="J82" s="11">
-        <v>0.900167220487955</v>
+        <v>0.90016722048795506</v>
       </c>
       <c r="K82" s="11">
-        <v>0.0322957396873804</v>
+        <v>3.22957396873804E-2</v>
       </c>
       <c r="L82" s="11">
-        <v>35.8774891512644</v>
+        <v>35.877489151264399</v>
       </c>
       <c r="M82" s="11">
         <v>1.66621431324751</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B83" s="11">
-        <v>0.00499999010935426</v>
+        <v>4.9999901093542602E-3</v>
       </c>
       <c r="C83" s="12">
-        <v>-153.250997924805</v>
+        <v>-153.25099792480501</v>
       </c>
       <c r="D83" s="12">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="E83" s="12">
         <v>-63.7509979248047</v>
       </c>
       <c r="F83" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G83" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H83" s="12">
-        <v>83.8000030517578</v>
+        <v>83.800003051757798</v>
       </c>
       <c r="I83" s="14">
-        <v>0.0346156539916992</v>
+        <v>3.4615653991699198E-2</v>
       </c>
       <c r="J83" s="11">
-        <v>3.75128981706872</v>
+        <v>3.7512898170687201</v>
       </c>
       <c r="K83" s="11">
-        <v>0.0241240391507541</v>
+        <v>2.41240391507541E-2</v>
       </c>
       <c r="L83" s="11">
         <v>6.43086520294632</v>
@@ -3581,12 +3612,12 @@
         <v>1.67393752325976</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B84" s="11">
-        <v>0.00800000037997961</v>
+        <v>8.0000003799796104E-3</v>
       </c>
       <c r="C84" s="12">
         <v>-108.15</v>
@@ -3595,48 +3626,48 @@
         <v>58.2</v>
       </c>
       <c r="E84" s="12">
-        <v>16.5500122070313</v>
+        <v>16.550012207031301</v>
       </c>
       <c r="F84" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G84" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H84" s="12">
-        <v>131.300003051758</v>
+        <v>131.30000305175801</v>
       </c>
       <c r="I84" s="14">
-        <v>0.0444689788818359</v>
+        <v>4.4468978881835902E-2</v>
       </c>
       <c r="J84" s="11">
-        <v>5.90381662461248</v>
+        <v>5.9038166246124799</v>
       </c>
       <c r="K84" s="11">
-        <v>0.0219931774924653</v>
+        <v>2.19931774924653E-2</v>
       </c>
       <c r="L84" s="11">
-        <v>3.72524739348741</v>
+        <v>3.7252473934874102</v>
       </c>
       <c r="M84" s="11">
-        <v>1.681927794409</v>
-      </c>
-    </row>
-    <row r="85">
+        <v>1.6819277944090001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B85" s="11">
-        <v>0.104070000350475</v>
+        <v>0.10407000035047501</v>
       </c>
       <c r="C85" s="12">
-        <v>46.2090087890625</v>
+        <v>46.209008789062501</v>
       </c>
       <c r="D85" s="12">
-        <v>79.0339013671875</v>
+        <v>79.033901367187497</v>
       </c>
       <c r="E85" s="12">
-        <v>278.85</v>
+        <v>278.85000000000002</v>
       </c>
       <c r="F85" s="13">
         <v>-1103.54775</v>
@@ -3645,75 +3676,75 @@
         <v>115.999</v>
       </c>
       <c r="H85" s="12">
-        <v>76.130500793457</v>
+        <v>76.130500793457003</v>
       </c>
       <c r="I85" s="14">
-        <v>0.0611599006652832</v>
+        <v>6.11599006652832E-2</v>
       </c>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B86" s="11">
-        <v>0.104070000350475</v>
+        <v>0.10407000035047501</v>
       </c>
       <c r="C86" s="12">
         <v>-50.15</v>
       </c>
       <c r="D86" s="12">
-        <v>61.7981005859375</v>
+        <v>61.798100585937497</v>
       </c>
       <c r="E86" s="12">
         <v>105.649011230469</v>
       </c>
       <c r="F86" s="13">
-        <v>-547.7021875</v>
+        <v>-547.70218750000004</v>
       </c>
       <c r="G86" s="13">
         <v>-142.04</v>
       </c>
       <c r="H86" s="12">
-        <v>60.0699005126953</v>
+        <v>60.069900512695298</v>
       </c>
       <c r="I86" s="14">
-        <v>0.062369800567627</v>
+        <v>6.2369800567626997E-2</v>
       </c>
       <c r="J86" s="11">
-        <v>2.72150092531717</v>
+        <v>2.7215009253171698</v>
       </c>
       <c r="K86" s="11">
-        <v>0.0110649832544801</v>
+        <v>1.1064983254480101E-2</v>
       </c>
       <c r="L86" s="11">
-        <v>4.06576501648279</v>
+        <v>4.0657650164827901</v>
       </c>
       <c r="M86" s="11">
-        <v>1.27574639117564</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>1.2757463911756399</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B87" s="11">
-        <v>0.833980023860931</v>
+        <v>0.83398002386093095</v>
       </c>
       <c r="C87" s="12">
-        <v>21.1490112304688</v>
+        <v>21.149011230468801</v>
       </c>
       <c r="D87" s="12">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="E87" s="12">
         <v>157.847009277344</v>
       </c>
       <c r="F87" s="13">
-        <v>-33.09530078125</v>
+        <v>-33.095300781250003</v>
       </c>
       <c r="G87" s="13">
         <v>33.869</v>
@@ -3722,22 +3753,22 @@
         <v>46.0060005187988</v>
       </c>
       <c r="I87" s="14">
-        <v>0.0319717826843262</v>
+        <v>3.1971782684326197E-2</v>
       </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B88" s="11">
-        <v>0.587970018386841</v>
+        <v>0.58797001838684104</v>
       </c>
       <c r="C88" s="12">
-        <v>-151.749998474121</v>
+        <v>-151.74999847412101</v>
       </c>
       <c r="D88" s="12">
         <v>64.7</v>
@@ -3746,10 +3777,10 @@
         <v>-93.15</v>
       </c>
       <c r="F88" s="13">
-        <v>-90.248703125</v>
+        <v>-90.248703125000006</v>
       </c>
       <c r="G88" s="13">
-        <v>90.427</v>
+        <v>90.427000000000007</v>
       </c>
       <c r="H88" s="12">
         <v>30.0060005187988</v>
@@ -3758,10 +3789,10 @@
         <v>0.420707580566406</v>
       </c>
       <c r="J88" s="11">
-        <v>1.33983373743984</v>
+        <v>1.3398337374398399</v>
       </c>
       <c r="K88" s="11">
-        <v>0.0208450312957117</v>
+        <v>2.0845031295711702E-2</v>
       </c>
       <c r="L88" s="11">
         <v>15.5579238775868</v>
@@ -3770,15 +3801,15 @@
         <v>1.39103556376675</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B89" s="11">
-        <v>0.256000012159348</v>
+        <v>0.25600001215934798</v>
       </c>
       <c r="C89" s="12">
-        <v>-9.94998779296873</v>
+        <v>-9.9499877929687308</v>
       </c>
       <c r="D89" s="12">
         <v>78.7</v>
@@ -3787,45 +3818,45 @@
         <v>157.649011230469</v>
       </c>
       <c r="F89" s="13">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G89" s="13">
-        <v>-297.1</v>
+        <v>-297.10000000000002</v>
       </c>
       <c r="H89" s="12">
-        <v>64.0630035400391</v>
+        <v>64.063003540039105</v>
       </c>
       <c r="I89" s="14">
-        <v>0.0489435920715332</v>
+        <v>4.8943592071533197E-2</v>
       </c>
       <c r="J89" s="11">
-        <v>2.91107746973666</v>
+        <v>2.9110774697366599</v>
       </c>
       <c r="K89" s="11">
-        <v>0.0107467800801502</v>
+        <v>1.07467800801502E-2</v>
       </c>
       <c r="L89" s="11">
-        <v>3.69168467410191</v>
+        <v>3.6916846741019098</v>
       </c>
       <c r="M89" s="11">
-        <v>1.28992266852493</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>1.2899226685249301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B90" s="11">
-        <v>0.0850000008940697</v>
+        <v>8.5000000894069699E-2</v>
       </c>
       <c r="C90" s="12">
-        <v>-103.750997924805</v>
+        <v>-103.75099792480501</v>
       </c>
       <c r="D90" s="12">
-        <v>50.317900390625</v>
+        <v>50.317900390624999</v>
       </c>
       <c r="E90" s="12">
-        <v>9.20900878906252</v>
+        <v>9.2090087890625192</v>
       </c>
       <c r="F90" s="13">
         <v>-1323.57</v>
@@ -3843,30 +3874,30 @@
         <v>1.26226920459595</v>
       </c>
       <c r="K90" s="11">
-        <v>0.00933238983867976</v>
+        <v>9.3323898386797593E-3</v>
       </c>
       <c r="L90" s="11">
-        <v>7.39334351555143</v>
+        <v>7.3933435155514298</v>
       </c>
       <c r="M90" s="11">
         <v>1.2537551748125</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B91" s="11">
-        <v>0.187270000576973</v>
+        <v>0.18727000057697299</v>
       </c>
       <c r="C91" s="12">
-        <v>-83.7999938964844</v>
+        <v>-83.799993896484395</v>
       </c>
       <c r="D91" s="12">
-        <v>61.3910009765625</v>
+        <v>61.391000976562502</v>
       </c>
       <c r="E91" s="12">
-        <v>35.1700073242188</v>
+        <v>35.170007324218801</v>
       </c>
       <c r="F91" s="13">
         <v>-1256.2</v>
@@ -3875,69 +3906,69 @@
         <v>226.9</v>
       </c>
       <c r="H91" s="12">
-        <v>26.0380001068115</v>
+        <v>26.038000106811499</v>
       </c>
       <c r="I91" s="14">
         <v>0.1024365234375</v>
       </c>
       <c r="J91" s="11">
-        <v>1.17221740987131</v>
+        <v>1.1722174098713101</v>
       </c>
       <c r="K91" s="11">
-        <v>0.00901056004092458</v>
+        <v>9.0105600409245805E-3</v>
       </c>
       <c r="L91" s="11">
-        <v>7.68676524085562</v>
+        <v>7.6867652408556202</v>
       </c>
       <c r="M91" s="11">
-        <v>1.24012848776221</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>1.2401284877622101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B92" s="11">
-        <v>0.215000003576279</v>
+        <v>0.21500000357627899</v>
       </c>
       <c r="C92" s="12">
-        <v>80.089013671875</v>
+        <v>80.089013671874994</v>
       </c>
       <c r="D92" s="12">
-        <v>49.2439013671875</v>
+        <v>49.243901367187497</v>
       </c>
       <c r="E92" s="12">
-        <v>288.948022460938</v>
+        <v>288.94802246093798</v>
       </c>
       <c r="F92" s="13">
         <v>-3170.97</v>
       </c>
       <c r="G92" s="13">
-        <v>82.977</v>
+        <v>82.977000000000004</v>
       </c>
       <c r="H92" s="12">
-        <v>78.1100006103516</v>
+        <v>78.110000610351605</v>
       </c>
       <c r="I92" s="14">
-        <v>0.0894000015258789</v>
+        <v>8.9400001525878903E-2</v>
       </c>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B93" s="11">
-        <v>0.259600013494492</v>
+        <v>0.25960001349449202</v>
       </c>
       <c r="C93" s="12">
         <v>110.649011230469</v>
       </c>
       <c r="D93" s="12">
-        <v>41.000400390625</v>
+        <v>41.000400390625003</v>
       </c>
       <c r="E93" s="12">
         <v>318.649011230469</v>
@@ -3946,28 +3977,28 @@
         <v>-3773.65</v>
       </c>
       <c r="G93" s="13">
-        <v>50.029</v>
+        <v>50.029000000000003</v>
       </c>
       <c r="H93" s="12">
-        <v>92.1408004760742</v>
+        <v>92.140800476074205</v>
       </c>
       <c r="I93" s="14">
-        <v>0.106800003051758</v>
+        <v>0.10680000305175801</v>
       </c>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B94" s="11">
-        <v>0.32600000500679</v>
+        <v>0.32600000500678999</v>
       </c>
       <c r="C94" s="12">
-        <v>139.115014648438</v>
+        <v>139.11501464843801</v>
       </c>
       <c r="D94" s="12">
         <v>35.411201171875</v>
@@ -3979,10 +4010,10 @@
         <v>-4376.54</v>
       </c>
       <c r="G94" s="13">
-        <v>17.249</v>
+        <v>17.248999999999999</v>
       </c>
       <c r="H94" s="12">
-        <v>106.166000366211</v>
+        <v>106.16600036621099</v>
       </c>
       <c r="I94" s="14">
         <v>0.1235</v>
@@ -3992,18 +4023,18 @@
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B95" s="11">
-        <v>0.302300006151199</v>
+        <v>0.30230000615119901</v>
       </c>
       <c r="C95" s="12">
-        <v>144.425012207031</v>
+        <v>144.42501220703099</v>
       </c>
       <c r="D95" s="12">
-        <v>37.3281005859375</v>
+        <v>37.328100585937499</v>
       </c>
       <c r="E95" s="12">
         <v>357.222009277344</v>
@@ -4012,10 +4043,10 @@
         <v>-4378.3</v>
       </c>
       <c r="G95" s="13">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="H95" s="12">
-        <v>106.166000366211</v>
+        <v>106.16600036621099</v>
       </c>
       <c r="I95" s="14">
         <v>0.121196998596191</v>
@@ -4025,51 +4056,51 @@
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B96" s="11">
-        <v>0.129960000514984</v>
+        <v>0.12996000051498399</v>
       </c>
       <c r="C96" s="12">
-        <v>-32.7789978027344</v>
+        <v>-32.778997802734402</v>
       </c>
       <c r="D96" s="12">
-        <v>54.95080078125</v>
+        <v>54.950800781250003</v>
       </c>
       <c r="E96" s="12">
         <v>124.661004638672</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="13">
-        <v>53.338</v>
+        <v>53.338000000000001</v>
       </c>
       <c r="H96" s="12">
-        <v>42.0806007385254</v>
+        <v>42.080600738525398</v>
       </c>
       <c r="I96" s="14">
-        <v>0.0681225891113281</v>
+        <v>6.8122589111328097E-2</v>
       </c>
       <c r="J96" s="11">
-        <v>1.91529737594189</v>
+        <v>1.9152973759418901</v>
       </c>
       <c r="K96" s="11">
-        <v>0.00799956221357561</v>
+        <v>7.9995622135756103E-3</v>
       </c>
       <c r="L96" s="11">
-        <v>4.17666849757034</v>
+        <v>4.1766684975703399</v>
       </c>
       <c r="M96" s="11">
-        <v>1.21602079646987</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>1.2160207964698699</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B97" s="11">
-        <v>0.148000001907349</v>
+        <v>0.14800000190734899</v>
       </c>
       <c r="C97" s="12">
         <v>-47.7509979248047</v>
@@ -4084,42 +4115,42 @@
         <v>-1927.35</v>
       </c>
       <c r="G97" s="13">
-        <v>20.429</v>
+        <v>20.428999999999998</v>
       </c>
       <c r="H97" s="12">
-        <v>42.0806007385254</v>
+        <v>42.080600738525398</v>
       </c>
       <c r="I97" s="14">
-        <v>0.079</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="J97" s="11">
-        <v>1.91358735948561</v>
+        <v>1.9135873594856101</v>
       </c>
       <c r="K97" s="11">
-        <v>0.00784407293191177</v>
+        <v>7.8440729319117705E-3</v>
       </c>
       <c r="L97" s="11">
-        <v>4.09914545736774</v>
+        <v>4.0991454573677402</v>
       </c>
       <c r="M97" s="11">
-        <v>1.17262130635451</v>
-      </c>
-    </row>
-    <row r="98">
+        <v>1.1726213063545099</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B98" s="11">
-        <v>0.325890004634857</v>
+        <v>0.32589000463485701</v>
       </c>
       <c r="C98" s="12">
-        <v>138.360009765625</v>
+        <v>138.36000976562499</v>
       </c>
       <c r="D98" s="12">
-        <v>35.107900390625</v>
+        <v>35.107900390624998</v>
       </c>
       <c r="E98" s="12">
-        <v>343.110009765625</v>
+        <v>343.11000976562502</v>
       </c>
       <c r="F98" s="13">
         <v>-4377.25</v>
@@ -4128,7 +4159,7 @@
         <v>17.95</v>
       </c>
       <c r="H98" s="12">
-        <v>106.166000366211</v>
+        <v>106.16600036621099</v>
       </c>
       <c r="I98" s="14">
         <v>0.124</v>
@@ -4138,30 +4169,30 @@
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B99" s="11">
-        <v>0.300980001688004</v>
+        <v>0.30098000168800398</v>
       </c>
       <c r="C99" s="12">
-        <v>136.200006103516</v>
+        <v>136.20000610351599</v>
       </c>
       <c r="D99" s="12">
-        <v>36.071201171875</v>
+        <v>36.071201171875003</v>
       </c>
       <c r="E99" s="12">
-        <v>343.948022460938</v>
+        <v>343.94802246093798</v>
       </c>
       <c r="F99" s="13">
-        <v>-4389.14</v>
+        <v>-4389.1400000000003</v>
       </c>
       <c r="G99" s="13">
-        <v>29.809</v>
+        <v>29.809000000000001</v>
       </c>
       <c r="H99" s="12">
-        <v>106.166000366211</v>
+        <v>106.16600036621099</v>
       </c>
       <c r="I99" s="14">
         <v>0.12309700012207</v>
@@ -4172,6 +4203,7 @@
       <c r="M99" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>